<commit_message>
Added munging script to create Th1/2/17 GatingSet. BSMS not included because it did not include CXCR3
</commit_message>
<xml_diff>
--- a/UCLA.xlsx
+++ b/UCLA.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28720" windowHeight="17560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28720" windowHeight="17560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Comp controls" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="99">
   <si>
     <t>Marker</t>
   </si>
@@ -308,6 +308,15 @@
   </si>
   <si>
     <t>Compensation Controls_HLA-DR BD Horizon V500-A Stained Control.fcs</t>
+  </si>
+  <si>
+    <t>TH 22013_1369_001.fcs</t>
+  </si>
+  <si>
+    <t>TH 22013_1369_002.fcs</t>
+  </si>
+  <si>
+    <t>TH 22013_1369_003.fcs</t>
   </si>
 </sst>
 </file>
@@ -815,7 +824,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1251,8 +1260,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1919,7 +1928,7 @@
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="1" t="s">
-        <v>28</v>
+        <v>96</v>
       </c>
       <c r="B46" s="8"/>
       <c r="C46" t="s">
@@ -1934,7 +1943,7 @@
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="1" t="s">
-        <v>29</v>
+        <v>97</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" t="s">
@@ -1949,7 +1958,7 @@
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="1" t="s">
-        <v>30</v>
+        <v>98</v>
       </c>
       <c r="B48" s="8"/>
       <c r="C48" t="s">

</xml_diff>